<commit_message>
update price list docs
</commit_message>
<xml_diff>
--- a/Docs/Robot Price List/Robot Price List.xlsx
+++ b/Docs/Robot Price List/Robot Price List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Canteiro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Canteiro\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C46CEF1-AF06-466C-AE6E-FF7C35AEF836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2859325-D357-4B9C-A736-D3C497373378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74353771-57BD-4A43-851A-534913C90AE0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
   <si>
     <t>Price</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>1 meter</t>
+  </si>
+  <si>
+    <t>3D Printed Stabilizer Parts</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2521A022-343D-4258-B40E-6452BD2433BF}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1117,7 +1120,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="20">
-        <f t="shared" ref="F4:F65" si="0">B4 * D4</f>
+        <f t="shared" ref="F4:F66" si="0">B4 * D4</f>
         <v>0.89</v>
       </c>
       <c r="G4" s="24" t="s">
@@ -2091,393 +2094,417 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="24"/>
+      <c r="A49" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="15">
+        <v>2.88</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="16">
+        <v>2</v>
+      </c>
+      <c r="E49" s="17">
+        <v>2</v>
+      </c>
+      <c r="F49" s="15">
+        <f t="shared" si="0"/>
+        <v>5.76</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="24"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B51" s="15">
         <v>8.93</v>
       </c>
-      <c r="C50" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="16">
-        <v>1</v>
-      </c>
-      <c r="E50" s="17">
-        <v>1</v>
-      </c>
-      <c r="F50" s="15">
+      <c r="C51" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="16">
+        <v>1</v>
+      </c>
+      <c r="E51" s="17">
+        <v>1</v>
+      </c>
+      <c r="F51" s="15">
         <f t="shared" si="0"/>
         <v>8.93</v>
       </c>
-      <c r="G50" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="19" t="s">
+      <c r="G51" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B52" s="20">
         <v>1.92</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="22">
-        <v>1</v>
-      </c>
-      <c r="E51" s="23">
-        <v>1</v>
-      </c>
-      <c r="F51" s="20">
+      <c r="C52" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="22">
+        <v>1</v>
+      </c>
+      <c r="E52" s="23">
+        <v>1</v>
+      </c>
+      <c r="F52" s="20">
         <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
-      <c r="G51" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="14"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="18"/>
+      <c r="G52" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="18"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="20">
+      <c r="B54" s="20">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D53" s="22">
+      <c r="C54" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="22">
         <v>14</v>
       </c>
-      <c r="E53" s="23">
+      <c r="E54" s="23">
         <v>14</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F54" s="20">
         <f t="shared" si="0"/>
         <v>1.3860000000000001</v>
       </c>
-      <c r="G53" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="14" t="s">
+      <c r="G54" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B55" s="15">
         <v>1.9E-2</v>
       </c>
-      <c r="C54" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="16">
+      <c r="C55" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="16">
         <v>26</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E55" s="17">
         <v>26</v>
       </c>
-      <c r="F54" s="15">
+      <c r="F55" s="15">
         <f t="shared" si="0"/>
         <v>0.49399999999999999</v>
       </c>
-      <c r="G54" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="19" t="s">
+      <c r="G55" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B56" s="20">
         <v>2.4E-2</v>
       </c>
-      <c r="C55" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="22">
+      <c r="C56" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="22">
         <v>4</v>
       </c>
-      <c r="E55" s="23">
+      <c r="E56" s="23">
         <v>4</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F56" s="20">
         <f t="shared" si="0"/>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="G55" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="14" t="s">
+      <c r="G56" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B57" s="15">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="C56" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="16">
+      <c r="C57" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="16">
         <v>30</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E57" s="17">
         <v>30</v>
       </c>
-      <c r="F56" s="15">
+      <c r="F57" s="15">
         <f t="shared" si="0"/>
         <v>1.1099999999999999</v>
       </c>
-      <c r="G56" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="19" t="s">
+      <c r="G57" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="20">
+      <c r="B58" s="20">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="C57" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" s="22">
+      <c r="C58" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="22">
         <v>2</v>
       </c>
-      <c r="E57" s="23">
+      <c r="E58" s="23">
         <v>2</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F58" s="20">
         <f t="shared" si="0"/>
         <v>0.104</v>
       </c>
-      <c r="G57" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="14" t="s">
+      <c r="G58" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B59" s="15">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="C58" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="16">
+      <c r="C59" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="16">
         <v>8</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E59" s="17">
         <v>8</v>
       </c>
-      <c r="F58" s="15">
+      <c r="F59" s="15">
         <f t="shared" si="0"/>
         <v>0.28799999999999998</v>
       </c>
-      <c r="G58" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="19" t="s">
+      <c r="G59" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="20">
+      <c r="B60" s="20">
         <v>2.3E-2</v>
       </c>
-      <c r="C59" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D59" s="22">
+      <c r="C60" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="22">
         <v>8</v>
       </c>
-      <c r="E59" s="23">
+      <c r="E60" s="23">
         <v>8</v>
       </c>
-      <c r="F59" s="20">
+      <c r="F60" s="20">
         <f t="shared" si="0"/>
         <v>0.184</v>
       </c>
-      <c r="G59" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="14" t="s">
+      <c r="G60" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B61" s="15">
         <v>3.42</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C61" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D61" s="16">
         <v>2</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E61" s="17">
         <v>51</v>
       </c>
-      <c r="F60" s="15">
+      <c r="F61" s="15">
         <f t="shared" si="0"/>
         <v>6.84</v>
       </c>
-      <c r="G60" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="19" t="s">
+      <c r="G61" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B62" s="20">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C61" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="22">
+      <c r="C62" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="22">
         <v>2</v>
       </c>
-      <c r="E61" s="23">
+      <c r="E62" s="23">
         <v>2</v>
       </c>
-      <c r="F61" s="20">
+      <c r="F62" s="20">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="G61" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="14" t="s">
+      <c r="G62" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B63" s="15">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C62" s="25" t="s">
+      <c r="C63" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="16">
-        <v>1</v>
-      </c>
-      <c r="E62" s="17">
+      <c r="D63" s="16">
+        <v>1</v>
+      </c>
+      <c r="E63" s="17">
         <v>8</v>
       </c>
-      <c r="F62" s="15">
+      <c r="F63" s="15">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="G62" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="19" t="s">
+      <c r="G63" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="20">
+      <c r="B64" s="20">
         <v>0.2</v>
       </c>
-      <c r="C63" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D63" s="22">
+      <c r="C64" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="22">
         <v>2</v>
       </c>
-      <c r="E63" s="23">
+      <c r="E64" s="23">
         <v>2</v>
       </c>
-      <c r="F63" s="20">
+      <c r="F64" s="20">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G63" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="14" t="s">
+      <c r="G64" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="15">
+      <c r="B65" s="15">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="C64" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" s="16">
+      <c r="C65" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="16">
         <v>6</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E65" s="17">
         <v>6</v>
       </c>
-      <c r="F64" s="15">
+      <c r="F65" s="15">
         <f t="shared" si="0"/>
         <v>0.21599999999999997</v>
       </c>
-      <c r="G64" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="34" t="s">
+      <c r="G65" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="35">
+      <c r="B66" s="35">
         <v>0.42</v>
       </c>
-      <c r="C65" s="36" t="s">
+      <c r="C66" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D65" s="37">
-        <v>1</v>
-      </c>
-      <c r="E65" s="38">
+      <c r="D66" s="37">
+        <v>1</v>
+      </c>
+      <c r="E66" s="38">
         <v>4</v>
       </c>
-      <c r="F65" s="35">
+      <c r="F66" s="35">
         <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
-      <c r="G65" s="39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="4" t="s">
+      <c r="G66" s="39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="5">
-        <f>SUM(F3:F200026)</f>
-        <v>279.57799999999997</v>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="5">
+        <f>SUM(F3:F200027)</f>
+        <v>285.33799999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2523,26 +2550,27 @@
     <hyperlink ref="G46" r:id="rId35" xr:uid="{2DA56BD8-9B8A-4FB1-8E28-8256482E5679}"/>
     <hyperlink ref="G47" r:id="rId36" xr:uid="{87ED82D9-CB33-4E98-8F02-7B17F66E9C5D}"/>
     <hyperlink ref="G48" r:id="rId37" xr:uid="{2577637C-60BB-4792-8018-DA153BE911D4}"/>
-    <hyperlink ref="G51" r:id="rId38" xr:uid="{3BA49FE9-306C-4929-A043-464DF5B7A951}"/>
-    <hyperlink ref="G50" r:id="rId39" xr:uid="{CD6E42A1-297E-4E25-803E-0ADA0F4627D1}"/>
-    <hyperlink ref="G56" r:id="rId40" xr:uid="{F954AD43-16CC-49CA-AE0D-C07970ED3DEF}"/>
-    <hyperlink ref="G60" r:id="rId41" xr:uid="{BFE7D769-36BE-4EBC-BC63-7DF7E8DDA493}"/>
-    <hyperlink ref="G61" r:id="rId42" xr:uid="{49B2452C-BBBA-45C2-896B-B19027812696}"/>
-    <hyperlink ref="G53" r:id="rId43" xr:uid="{BFC7914F-6C11-4731-AE07-CDF03404907B}"/>
-    <hyperlink ref="G54" r:id="rId44" xr:uid="{D57EE8D8-78E3-466E-85D9-9DBF539459E1}"/>
-    <hyperlink ref="G64" r:id="rId45" xr:uid="{E173C34F-53C3-4562-9A7E-97C9584C46AC}"/>
-    <hyperlink ref="G62" r:id="rId46" xr:uid="{7B82CC86-4AAE-4AF7-A8BE-1CEDB874FE1B}"/>
-    <hyperlink ref="G65" r:id="rId47" xr:uid="{F20C5E10-A2A6-465B-8B82-D193AB17F4BC}"/>
-    <hyperlink ref="G55" r:id="rId48" xr:uid="{947C89E0-9DFF-4D66-8C10-A31E78412699}"/>
-    <hyperlink ref="G57" r:id="rId49" xr:uid="{3DF59D61-C025-46DD-97DC-C2A240E9A7E6}"/>
+    <hyperlink ref="G52" r:id="rId38" xr:uid="{3BA49FE9-306C-4929-A043-464DF5B7A951}"/>
+    <hyperlink ref="G51" r:id="rId39" xr:uid="{CD6E42A1-297E-4E25-803E-0ADA0F4627D1}"/>
+    <hyperlink ref="G57" r:id="rId40" xr:uid="{F954AD43-16CC-49CA-AE0D-C07970ED3DEF}"/>
+    <hyperlink ref="G61" r:id="rId41" xr:uid="{BFE7D769-36BE-4EBC-BC63-7DF7E8DDA493}"/>
+    <hyperlink ref="G62" r:id="rId42" xr:uid="{49B2452C-BBBA-45C2-896B-B19027812696}"/>
+    <hyperlink ref="G54" r:id="rId43" xr:uid="{BFC7914F-6C11-4731-AE07-CDF03404907B}"/>
+    <hyperlink ref="G55" r:id="rId44" xr:uid="{D57EE8D8-78E3-466E-85D9-9DBF539459E1}"/>
+    <hyperlink ref="G65" r:id="rId45" xr:uid="{E173C34F-53C3-4562-9A7E-97C9584C46AC}"/>
+    <hyperlink ref="G63" r:id="rId46" xr:uid="{7B82CC86-4AAE-4AF7-A8BE-1CEDB874FE1B}"/>
+    <hyperlink ref="G66" r:id="rId47" xr:uid="{F20C5E10-A2A6-465B-8B82-D193AB17F4BC}"/>
+    <hyperlink ref="G56" r:id="rId48" xr:uid="{947C89E0-9DFF-4D66-8C10-A31E78412699}"/>
+    <hyperlink ref="G58" r:id="rId49" xr:uid="{3DF59D61-C025-46DD-97DC-C2A240E9A7E6}"/>
     <hyperlink ref="G20" r:id="rId50" xr:uid="{5EB3D5AC-FF6F-4E40-9C1A-AC991712CA35}"/>
-    <hyperlink ref="G63" r:id="rId51" xr:uid="{AC772877-CECD-4902-84E5-5EA2A5C469E3}"/>
-    <hyperlink ref="G58" r:id="rId52" xr:uid="{C0942F39-B223-4302-A4E8-90FBD63AF593}"/>
-    <hyperlink ref="G59" r:id="rId53" xr:uid="{9631EE68-861B-4B9F-9993-BBA2BCEA8264}"/>
+    <hyperlink ref="G64" r:id="rId51" xr:uid="{AC772877-CECD-4902-84E5-5EA2A5C469E3}"/>
+    <hyperlink ref="G59" r:id="rId52" xr:uid="{C0942F39-B223-4302-A4E8-90FBD63AF593}"/>
+    <hyperlink ref="G60" r:id="rId53" xr:uid="{9631EE68-861B-4B9F-9993-BBA2BCEA8264}"/>
     <hyperlink ref="G37" r:id="rId54" xr:uid="{E8945C1D-22CA-4459-9DB5-7136582FA500}"/>
     <hyperlink ref="G38" r:id="rId55" xr:uid="{027C61B3-F753-49EB-997E-DCB99F45D6C3}"/>
+    <hyperlink ref="G49" r:id="rId56" xr:uid="{FF0C07E4-32F4-447E-B9A3-20DFF95C4A37}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>